<commit_message>
Calculate residuals, inventories, integrated fluxes, timescales for GP15
Also make section plots of the integrated fluxes for the NA inversion. PPZ for Station 1 was changed to 36m, was incorrect at 16m.
</commit_message>
<xml_diff>
--- a/data/gp15_ppz.xlsx
+++ b/data/gp15_ppz.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/particle/Library/Caches/com.binarynights.ForkLift2/#3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/particle/Library/Caches/com.binarynights.ForkLift2/#81/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D0128E-B215-2049-B134-1D85F9E11852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C38EFCA-2EE5-6F4B-8432-A3E04C028D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -450,7 +450,7 @@
   <dimension ref="A1:W997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -507,7 +507,7 @@
         <v>-156.96216000000001</v>
       </c>
       <c r="E2" s="1">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -542,7 +542,7 @@
         <v>-156.96270000000001</v>
       </c>
       <c r="E3" s="1">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>

</xml_diff>